<commit_message>
updates to datadriven utility piece for reading Excel files
</commit_message>
<xml_diff>
--- a/src/excelExportAndFileIO/dataExcel.xlsx
+++ b/src/excelExportAndFileIO/dataExcel.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26819"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-29700" yWindow="2500" windowWidth="28800" windowHeight="16640" tabRatio="500"/>
+    <workbookView xWindow="-32520" yWindow="3660" windowWidth="28840" windowHeight="16640" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="QA_Worksheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="45">
   <si>
     <t>CategoryName</t>
   </si>
@@ -33,12 +34,6 @@
     <t>I am having Download issues</t>
   </si>
   <si>
-    <t>http://test.com</t>
-  </si>
-  <si>
-    <t>http://anothertest.com</t>
-  </si>
-  <si>
     <t>TestCaseName</t>
   </si>
   <si>
@@ -61,6 +56,105 @@
   </si>
   <si>
     <t>Join Page Trying to Join Article 3 Test</t>
+  </si>
+  <si>
+    <t>http://support.citrixonline.com/en_US/Webinar/all_files/G2W090002?__col_mkt_cookies=__col_visit</t>
+  </si>
+  <si>
+    <t>http://support.citrixonline.com/en_US/Webinar/all_files/G2W030004?__col_mkt_cookies=__col_visit</t>
+  </si>
+  <si>
+    <t>Join Page - Trying to Join - Article 1 Test</t>
+  </si>
+  <si>
+    <t>Join Page - Trying to Join - Article 2 Test</t>
+  </si>
+  <si>
+    <t>Join Page - Trying to Join - Article 3 Test</t>
+  </si>
+  <si>
+    <t>Join Page - Trying to Join - Article 4 Test</t>
+  </si>
+  <si>
+    <t>Join Page - Trying to Join - Article 5 Test</t>
+  </si>
+  <si>
+    <t>Join Page - Trying to Join - Article 6 Test</t>
+  </si>
+  <si>
+    <t>Join Page - During Your Webinar - Article 1 Test</t>
+  </si>
+  <si>
+    <t>Join Page - During Your Webinar - Article 2 Test</t>
+  </si>
+  <si>
+    <t>Join Page - During Your Webinar - Article 3 Test</t>
+  </si>
+  <si>
+    <t>Join Page - During Your Webinar - Article 4 Test</t>
+  </si>
+  <si>
+    <t>Join Page - During Your Webinar - Article 5 Test</t>
+  </si>
+  <si>
+    <t>Join Page - During Your Webinar - Article 6 Test</t>
+  </si>
+  <si>
+    <t>During Your Webinar</t>
+  </si>
+  <si>
+    <t>How do I install GoToWebinar on a Mac?</t>
+  </si>
+  <si>
+    <t>How do I install GoToWebinar on a PC?</t>
+  </si>
+  <si>
+    <t>I'm still having trouble joining - what else can I try?</t>
+  </si>
+  <si>
+    <t>http://support.citrixonline.com/en_US/Webinar/help_files/G2W060005?__col_mkt_cookies=__col_visit</t>
+  </si>
+  <si>
+    <t>http://support.citrixonline.com/en_US/Webinar/help_files/G2W060021?__col_mkt_cookies=__col_visit</t>
+  </si>
+  <si>
+    <t>http://support.citrixonline.com/en_US/webinar/all_files/G2W060007?__col_mkt_cookies=__col_visit</t>
+  </si>
+  <si>
+    <t>https://support.citrixonline.com/en_US/webinar/knowledge_articles/000025306?__col_mkt_cookies=__col_visit</t>
+  </si>
+  <si>
+    <t>I registered for the webinar but now I see "The session is full"</t>
+  </si>
+  <si>
+    <t>I can only hear the audio or see the screen, but not both</t>
+  </si>
+  <si>
+    <t>It says I've connected, but the webinar isn't started</t>
+  </si>
+  <si>
+    <t>How do I unmute myself?</t>
+  </si>
+  <si>
+    <t>Why can't anyone hear me?</t>
+  </si>
+  <si>
+    <t>I have a question or feedback about the presentation itself (materials, certification, etc.)</t>
+  </si>
+  <si>
+    <t>http://support.citrixonline.com/en_US/webinar/help_files/G2W090003?__col_mkt_cookies=__col_visit</t>
+  </si>
+  <si>
+    <t>http://support.citrixonline.com/en_US/webinar/knowledge_articles/000161527?title=Waiting+for+Organizer&amp;__col_mkt_cookies=__col_visit</t>
+  </si>
+  <si>
+    <t>http://support.citrixonline.com/en_US/Webinar/all_files/G2W050039?__col_mkt_cookies=__col_visit</t>
+  </si>
+  <si>
+    <t>http://support.citrixonline.com/en_US/Webinar/all_files/G2W050053?__col_mkt_cookies=__col_visit</t>
+  </si>
+  <si>
+    <t>https://support.citrixonline.com/en_US/webinar/knowledge_articles/000064729?__col_mkt_cookies=__col_visit</t>
   </si>
 </sst>
 </file>
@@ -502,43 +596,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="31.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="104.5" customWidth="1"/>
-    <col min="4" max="4" width="39.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.5" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="117" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>1</v>
@@ -546,13 +640,13 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
         <v>12</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>4</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>2</v>
@@ -560,22 +654,147 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
         <v>13</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>5</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1"/>
-    <hyperlink ref="C4" r:id="rId2"/>
+    <hyperlink ref="C5" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -585,4 +804,84 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="31.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>